<commit_message>
coding SRI + R script eye tracking data + subject list
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/SRI/Kodierschema_SRI.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/SRI/Kodierschema_SRI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\studies\Laborstudie ProVisioNET\SRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\SRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{93D9C11F-97CD-4256-BCE3-FEB19CA4E8AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C135E16D-8E7D-4EFE-BF7E-0ABE53222BBA}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{93D9C11F-97CD-4256-BCE3-FEB19CA4E8AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0E3BE09D-F930-4FD4-B24A-A3F18C417343}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11220" xr2:uid="{ECFD9030-D81A-4832-8358-84AEA871CE62}"/>
   </bookViews>
@@ -992,9 +992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3636F8-4881-41FE-AA30-7E39DF0AE8CB}">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>